<commit_message>
update extracteur temps moyen
</commit_message>
<xml_diff>
--- a/front/src/assets/template2.xlsx
+++ b/front/src/assets/template2.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E23E1ED-6E61-134B-B978-EE09342AD01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A12AFB-1700-D046-8C58-DDD96A0B7C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="14560" xr2:uid="{78BE7E27-F763-E84B-A118-EEDD18AEE1B3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" xr2:uid="{78BE7E27-F763-E84B-A118-EEDD18AEE1B3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MAGISTRATS" sheetId="2" r:id="rId1"/>
+    <sheet name="FONCTIONNAIRES" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FONCTIONNAIRES!$A$2:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MAGISTRATS!$A$2:$D$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +32,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,60 +41,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
-  <si>
-    <t>Valid template</t>
-  </si>
-  <si>
-    <t>#` I am ${author.firstName} ${author.lastName} ,  and my hobby is ${author.hobby}</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Invalid template (wrong paths)</t>
-  </si>
-  <si>
-    <t>Invalid template (brackets)</t>
-  </si>
-  <si>
-    <t>Invalid template (## instead of #`)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ## I am ${author.first{Name} ${author.last}Name} ,  and my hobby is ${author.hobby}</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> #` I am ${author.firstName} ${author.lastName} ,  and my hobby is ${author.hobby}</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> #` I am ${a.u.t.hor.firs.t.Name} ${au.thor.la.stName} ,  and my hobby is ${au.thor.hob.by}</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> #` I am ${author.first{Name} ${author.last}Name} ,  and my hobby is ${author.hobby}</t>
-  </si>
-  <si>
-    <t>#` I am ${a.u.t.hor.firs.t.Name} ${au.thor.la.stName} ,  and my hobby is ${au.thor.hob.by}</t>
-  </si>
-  <si>
-    <t>#` I am ${author.first{Name} ${author.last}Name} ,  and my hobby is ${author.hobby}</t>
-  </si>
-  <si>
-    <t>## I am ${author.first{Name} ${author.last}Name} ,  and my hobby is ${author.hobby}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>#! END_ROW</t>
   </si>
   <si>
     <t>#! FINISH</t>
+  </si>
+  <si>
+    <t>#! CONTINUE w</t>
+  </si>
+  <si>
+    <t>#! END_LOOP w</t>
+  </si>
+  <si>
+    <t>Temps moyens en heures/minutes</t>
+  </si>
+  <si>
+    <t>Nombre de dossiers par jour</t>
+  </si>
+  <si>
+    <t>Nombre de dossiers par mois</t>
+  </si>
+  <si>
+    <t>Contentieux</t>
+  </si>
+  <si>
+    <t>## w.label</t>
+  </si>
+  <si>
+    <t>#! FOR_EACH w referentiels</t>
+  </si>
+  <si>
+    <t>#` ${name}</t>
+  </si>
+  <si>
+    <t>#! CONTINUE x</t>
+  </si>
+  <si>
+    <t>#! END_LOOP x</t>
+  </si>
+  <si>
+    <t>## x.averageProcessingTime</t>
+  </si>
+  <si>
+    <t>## x.label</t>
+  </si>
+  <si>
+    <t>#` ${nameFonc}</t>
+  </si>
+  <si>
+    <t>#! FOR_EACH x referentielsFonc</t>
+  </si>
+  <si>
+    <t>## x.nbPerDay</t>
+  </si>
+  <si>
+    <t>## x.nbPerMonth</t>
+  </si>
+  <si>
+    <t>## w.nbPerMonthFonc</t>
+  </si>
+  <si>
+    <t>## w.nbPerDayFonc</t>
+  </si>
+  <si>
+    <t>## w.averageProcessingTimeFonc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.###;0.###;\-"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -101,22 +126,22 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,24 +150,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -150,31 +169,27 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,94 +504,183 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D41A10BF-28E2-2848-A82B-175CECC31008}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9185C733-D2C4-5945-84AD-4FF37322E29A}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" customWidth="1"/>
-    <col min="2" max="2" width="78.83203125" customWidth="1"/>
-    <col min="3" max="3" width="76.33203125" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="4" width="21.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:D2" xr:uid="{9185C733-D2C4-5945-84AD-4FF37322E29A}"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9686D620-04EC-3340-83C1-86785DC7D7D0}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="4" width="21.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C1" xr:uid="{D41A10BF-28E2-2848-A82B-175CECC31008}"/>
+  <autoFilter ref="A2:D2" xr:uid="{9686D620-04EC-3340-83C1-86785DC7D7D0}"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update export excel temps moyen
</commit_message>
<xml_diff>
--- a/front/src/assets/template2.xlsx
+++ b/front/src/assets/template2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A12AFB-1700-D046-8C58-DDD96A0B7C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED8E53E-68E7-3244-B6E4-F0EC9F43F6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" xr2:uid="{78BE7E27-F763-E84B-A118-EEDD18AEE1B3}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>## x.nbPerDay</t>
-  </si>
-  <si>
-    <t>## x.nbPerMonth</t>
   </si>
   <si>
     <t>## w.nbPerMonthFonc</t>
@@ -141,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +154,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,11 +187,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -508,23 +513,23 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
-    <col min="2" max="4" width="21.83203125" style="4" customWidth="1"/>
+    <col min="2" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -550,15 +555,13 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="D3" s="6"/>
       <c r="E3" t="s">
         <v>11</v>
       </c>
@@ -567,15 +570,13 @@
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="D4" s="6"/>
       <c r="E4" t="s">
         <v>12</v>
       </c>
@@ -605,17 +606,17 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
-    <col min="2" max="4" width="21.83203125" style="4" customWidth="1"/>
+    <col min="2" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -641,14 +642,14 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -658,14 +659,14 @@
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>

</xml_diff>